<commit_message>
Add New Akuntansi Setup Up To TC 9
</commit_message>
<xml_diff>
--- a/DPLKADM003-035 - Setup Sumber Dana - Tambah, Ubah, View Detil & Hapus Data/Default.xlsx
+++ b/DPLKADM003-035 - Setup Sumber Dana - Tambah, Ubah, View Detil & Hapus Data/Default.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
-    <sheet name="ADM003-034" sheetId="2" r:id="rId2"/>
+    <sheet name="ADM003-035" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -183,10 +183,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="FFFFFF"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="283845"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>

</xml_diff>